<commit_message>
old recipe implementation to new. (using ingredients)
</commit_message>
<xml_diff>
--- a/sheets/Food System Design.xlsx
+++ b/sheets/Food System Design.xlsx
@@ -62,10 +62,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Weight by meat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Chicken</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -283,6 +279,10 @@
   </si>
   <si>
     <t>Pumpkin/melon seeds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Weight of meat</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -696,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:F54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -719,10 +719,10 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="J1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
@@ -730,16 +730,16 @@
         <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
@@ -750,13 +750,13 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3">
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K3">
         <f>L3*M3</f>
@@ -778,13 +778,13 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4">
         <v>5</v>
       </c>
       <c r="J4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K4">
         <f>L4*M4</f>
@@ -806,13 +806,13 @@
         <v>100</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5">
         <v>10</v>
       </c>
       <c r="J5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K5">
         <f>L5*M5</f>
@@ -839,7 +839,7 @@
         <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K6">
         <f>9*K3</f>
@@ -861,13 +861,13 @@
         <v>200</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G7">
         <v>15</v>
       </c>
       <c r="J7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K7">
         <f>M7*L7</f>
@@ -882,13 +882,13 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8">
         <v>200</v>
       </c>
       <c r="J8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K8">
         <f>M8*L8</f>
@@ -909,7 +909,7 @@
         <v>500</v>
       </c>
       <c r="J9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K9">
         <f>K4</f>
@@ -932,22 +932,22 @@
         <v>500</v>
       </c>
       <c r="J10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K10">
         <f>L10*M10</f>
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="L10" s="2">
         <v>0.25</v>
       </c>
       <c r="M10">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11">
         <f>(C7+C10)/2</f>
@@ -956,27 +956,27 @@
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" t="s">
         <v>37</v>
       </c>
-      <c r="C18" t="s">
+      <c r="E18" t="s">
         <v>57</v>
       </c>
-      <c r="D18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" t="s">
-        <v>58</v>
-      </c>
       <c r="G18" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" t="s">
         <v>55</v>
-      </c>
-      <c r="H18" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
@@ -1013,7 +1013,7 @@
         <v>5.9813951248848838</v>
       </c>
       <c r="D20">
-        <f t="shared" ref="D20:D21" si="0">C20/B20</f>
+        <f t="shared" ref="D20" si="0">C20/B20</f>
         <v>5.9813951248848835E-2</v>
       </c>
       <c r="E20">
@@ -1105,29 +1105,29 @@
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" t="s">
         <v>17</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>18</v>
-      </c>
-      <c r="D25" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" t="s">
         <v>15</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>16</v>
-      </c>
-      <c r="D26" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
@@ -1137,7 +1137,7 @@
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
@@ -1147,21 +1147,21 @@
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C37" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" t="s">
         <v>48</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>49</v>
-      </c>
-      <c r="E37" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.3">
@@ -1182,24 +1182,24 @@
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D41" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" t="s">
         <v>29</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>30</v>
-      </c>
-      <c r="F41" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
@@ -1228,17 +1228,17 @@
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C47">
         <v>0.3</v>
@@ -1246,7 +1246,7 @@
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -1254,26 +1254,26 @@
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C52" t="s">
+        <v>44</v>
+      </c>
+      <c r="D52" t="s">
         <v>45</v>
       </c>
-      <c r="D52" t="s">
-        <v>46</v>
-      </c>
       <c r="E52" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F52" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -1292,7 +1292,7 @@
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C54">
         <v>1.5</v>

</xml_diff>

<commit_message>
Add weight condition to courtship update
</commit_message>
<xml_diff>
--- a/sheets/Food System Design.xlsx
+++ b/sheets/Food System Design.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
   <si>
     <t xml:space="preserve">Base Weight </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -283,6 +283,10 @@
   </si>
   <si>
     <t>Weight of meat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stomach (kg)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -697,7 +701,7 @@
   <dimension ref="B1:M54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -972,6 +976,9 @@
       <c r="E18" t="s">
         <v>57</v>
       </c>
+      <c r="F18" t="s">
+        <v>65</v>
+      </c>
       <c r="G18" t="s">
         <v>54</v>
       </c>
@@ -995,6 +1002,10 @@
         <f>C19*$K$4/$L$4/(20*60)</f>
         <v>3.5455305979633267E-4</v>
       </c>
+      <c r="F19">
+        <f xml:space="preserve"> 20*60*G19</f>
+        <v>1.2763910152667977</v>
+      </c>
       <c r="G19">
         <f>1.2*C19/(20*60)</f>
         <v>1.063659179388998E-3</v>
@@ -1020,12 +1031,16 @@
         <f>C20*$K$4/$L$4/(20*60)</f>
         <v>1.9937983749616279E-3</v>
       </c>
+      <c r="F20">
+        <f t="shared" ref="F20:F23" si="1" xml:space="preserve"> 20*60*G20</f>
+        <v>7.1776741498618604</v>
+      </c>
       <c r="G20">
         <f>1.2*C20/(20*60)</f>
         <v>5.9813951248848833E-3</v>
       </c>
       <c r="H20">
-        <f t="shared" ref="H20:H23" si="1">B20/2/E20/(60*20)</f>
+        <f t="shared" ref="H20:H23" si="2">B20/2/E20/(60*20)</f>
         <v>20.898134530513182</v>
       </c>
     </row>
@@ -1045,12 +1060,16 @@
         <f>C21*$K$4/$L$4/(20*60)</f>
         <v>3.3531558124878292E-3</v>
       </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>12.071360924956183</v>
+      </c>
       <c r="G21">
         <f>1.2*C21/(20*60)</f>
         <v>1.0059467437463486E-2</v>
       </c>
       <c r="H21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24.852210273970321</v>
       </c>
     </row>
@@ -1070,12 +1089,16 @@
         <f>C22*$K$4/$L$4/(20*60)</f>
         <v>5.1019038650024365E-3</v>
       </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>18.366853914008768</v>
+      </c>
       <c r="G22">
         <f>1.2*C22/(20*60)</f>
         <v>1.5305711595007307E-2</v>
       </c>
       <c r="H22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28.584100600896697</v>
       </c>
     </row>
@@ -1094,12 +1117,16 @@
         <f>C23*$K$4/$L$4/(20*60)</f>
         <v>6.6666666666666671E-3</v>
       </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
       <c r="G23">
         <f>1.2*C23/(20*60)</f>
         <v>0.02</v>
       </c>
       <c r="H23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>31.25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add hay_block to item preferences.
</commit_message>
<xml_diff>
--- a/sheets/Food System Design.xlsx
+++ b/sheets/Food System Design.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="82">
   <si>
     <t xml:space="preserve">Base Weight </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -343,6 +343,14 @@
   </si>
   <si>
     <t>days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mixed feed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>straw</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -757,7 +765,7 @@
   <dimension ref="B1:N66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1015,6 +1023,36 @@
         <f>(C7+C10)/2</f>
         <v>350</v>
       </c>
+      <c r="J11" t="s">
+        <v>80</v>
+      </c>
+      <c r="K11">
+        <f>L11*M11</f>
+        <v>0.8</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J12" t="s">
+        <v>81</v>
+      </c>
+      <c r="K12">
+        <f>K3-2*K5</f>
+        <v>0.24999999999999989</v>
+      </c>
+      <c r="L12">
+        <f>L3-2*L5</f>
+        <v>0.54999999999999993</v>
+      </c>
+      <c r="M12">
+        <f>K12/L12</f>
+        <v>0.45454545454545442</v>
+      </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B14" t="s">

</xml_diff>

<commit_message>
Fix Resource Path Bug
</commit_message>
<xml_diff>
--- a/sheets/Food System Design.xlsx
+++ b/sheets/Food System Design.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
   <si>
     <t xml:space="preserve">Base Weight </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -351,6 +352,18 @@
   </si>
   <si>
     <t>straw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wolf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Carnivore</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ocelot</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -764,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -870,10 +883,10 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="C5">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
@@ -897,10 +910,10 @@
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
       <c r="C6">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F6" t="s">
         <v>4</v>
@@ -925,10 +938,10 @@
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
@@ -952,10 +965,10 @@
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="J8" t="s">
         <v>60</v>
@@ -973,10 +986,10 @@
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="J9" t="s">
         <v>61</v>
@@ -996,10 +1009,10 @@
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="C10">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="J10" t="s">
         <v>62</v>
@@ -1017,11 +1030,10 @@
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="C11">
-        <f>(C7+C10)/2</f>
-        <v>350</v>
+        <v>500</v>
       </c>
       <c r="J11" t="s">
         <v>80</v>
@@ -1038,6 +1050,12 @@
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>500</v>
+      </c>
       <c r="J12" t="s">
         <v>81</v>
       </c>
@@ -1054,19 +1072,16 @@
         <v>0.45454545454545442</v>
       </c>
     </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13">
+        <f>(C9+C12)/2</f>
+        <v>350</v>
+      </c>
+    </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14">
-        <v>2</v>
-      </c>
-      <c r="H14" t="s">
-        <v>72</v>
-      </c>
       <c r="K14" t="s">
         <v>75</v>
       </c>
@@ -1076,22 +1091,22 @@
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>83</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>68</v>
-      </c>
-      <c r="F15" t="s">
-        <v>69</v>
+        <v>67</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
       </c>
       <c r="H15" t="s">
-        <v>71</v>
-      </c>
-      <c r="I15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K15" t="s">
         <v>71</v>
@@ -1107,32 +1122,29 @@
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16">
-        <v>10</v>
-      </c>
-      <c r="C16">
-        <f>20*60*F16</f>
-        <v>1.5954887690834971</v>
-      </c>
-      <c r="E16">
-        <v>10</v>
-      </c>
-      <c r="F16">
-        <f>$F$14*C31/(20*60)</f>
-        <v>1.3295739742362476E-3</v>
-      </c>
-      <c r="H16">
-        <v>10</v>
-      </c>
-      <c r="I16">
-        <f>0.1*H16</f>
-        <v>1</v>
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16" t="s">
+        <v>71</v>
+      </c>
+      <c r="I16" t="s">
+        <v>73</v>
       </c>
       <c r="K16">
         <v>10</v>
       </c>
       <c r="L16">
-        <f>$L$14*(I16/2)/(F16*0.5-E31)</f>
+        <f>$L$14*(I17/2)/(F17*0.5-E31)</f>
         <v>2507.0687287242617</v>
       </c>
       <c r="M16">
@@ -1146,157 +1158,201 @@
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="C17">
-        <f t="shared" ref="C17:C20" si="0">20*60*F17</f>
-        <v>8.9720926873273257</v>
+        <f>20*60*F17</f>
+        <v>1.5954887690834971</v>
       </c>
       <c r="E17">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F17">
-        <f t="shared" ref="F17:F20" si="1">$F$14*C32/(20*60)</f>
-        <v>7.4767439061061043E-3</v>
+        <f>$F$15*C31/(20*60)</f>
+        <v>1.3295739742362476E-3</v>
       </c>
       <c r="H17">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="I17">
-        <f t="shared" ref="I17:I20" si="2">0.1*H17</f>
-        <v>10</v>
+        <f>0.1*H17</f>
+        <v>1</v>
       </c>
       <c r="K17">
         <v>100</v>
       </c>
       <c r="L17">
-        <f t="shared" ref="L17:L20" si="3">$L$14*(I17/2)/(F17*0.5-E32)</f>
+        <f>$L$14*(I19/2)/(F19*0.5-E33)</f>
         <v>4458.2686998428126</v>
       </c>
       <c r="M17">
-        <f t="shared" ref="M17:M20" si="4">20*L17</f>
+        <f t="shared" ref="M17:M20" si="0">20*L17</f>
         <v>89165.373996856244</v>
       </c>
       <c r="N17">
-        <f t="shared" ref="N17:N20" si="5">M17/24000</f>
+        <f t="shared" ref="N17:N20" si="1">M17/24000</f>
         <v>3.7152239165356766</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
-        <v>15.089201156195228</v>
+        <f>20*60*F18</f>
+        <v>5.3348382301167696</v>
       </c>
       <c r="E18">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="F18">
-        <f t="shared" si="1"/>
-        <v>1.2574334296829357E-2</v>
+        <f>$F$15*C32/(20*60)</f>
+        <v>4.4456985250973082E-3</v>
       </c>
       <c r="H18">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="I18">
-        <f t="shared" si="2"/>
-        <v>20</v>
+        <f>0.1*H18</f>
+        <v>5</v>
       </c>
       <c r="K18">
         <v>200</v>
       </c>
       <c r="L18">
-        <f t="shared" si="3"/>
+        <f>$L$14*(I20/2)/(F20*0.5-E34)</f>
         <v>5301.8048584470034</v>
       </c>
       <c r="M18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>106036.09716894006</v>
       </c>
       <c r="N18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>4.4181707153725025</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19">
-        <v>350</v>
+        <v>100</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
-        <v>22.958567392510961</v>
+        <f t="shared" ref="C19:C22" si="2">20*60*F19</f>
+        <v>8.9720926873273257</v>
       </c>
       <c r="E19">
-        <v>350</v>
+        <v>100</v>
       </c>
       <c r="F19">
-        <f t="shared" si="1"/>
-        <v>1.9132139493759134E-2</v>
+        <f>$F$15*C33/(20*60)</f>
+        <v>7.4767439061061043E-3</v>
       </c>
       <c r="H19">
-        <v>350</v>
+        <v>100</v>
       </c>
       <c r="I19">
-        <f t="shared" si="2"/>
-        <v>35</v>
+        <f t="shared" ref="I19:I22" si="3">0.1*H19</f>
+        <v>10</v>
       </c>
       <c r="K19">
         <v>350</v>
       </c>
       <c r="L19">
-        <f t="shared" si="3"/>
+        <f>$L$14*(I21/2)/(F21*0.5-E35)</f>
         <v>6097.9414615246296</v>
       </c>
       <c r="M19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>121958.82923049259</v>
       </c>
       <c r="N19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>5.0816178846038573</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
-        <v>30</v>
+        <f t="shared" si="2"/>
+        <v>15.089201156195228</v>
       </c>
       <c r="E20">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="F20">
-        <f t="shared" si="1"/>
-        <v>2.5000000000000001E-2</v>
+        <f>$F$15*C34/(20*60)</f>
+        <v>1.2574334296829357E-2</v>
       </c>
       <c r="H20">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="I20">
-        <f t="shared" si="2"/>
-        <v>50</v>
+        <f t="shared" si="3"/>
+        <v>20</v>
       </c>
       <c r="K20">
         <v>500</v>
       </c>
       <c r="L20">
+        <f>$L$14*(I22/2)/(F22*0.5-E36)</f>
+        <v>6666.6666666666661</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="0"/>
+        <v>133333.33333333331</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="1"/>
+        <v>5.5555555555555545</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>350</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="2"/>
+        <v>22.958567392510961</v>
+      </c>
+      <c r="E21">
+        <v>350</v>
+      </c>
+      <c r="F21">
+        <f>$F$15*C35/(20*60)</f>
+        <v>1.9132139493759134E-2</v>
+      </c>
+      <c r="H21">
+        <v>350</v>
+      </c>
+      <c r="I21">
         <f t="shared" si="3"/>
-        <v>6666.6666666666661</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="4"/>
-        <v>133333.33333333331</v>
-      </c>
-      <c r="N20">
-        <f t="shared" si="5"/>
-        <v>5.5555555555555545</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>500</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="E22">
+        <v>500</v>
+      </c>
+      <c r="F22">
+        <f>$F$15*C36/(20*60)</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H22">
+        <v>500</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
       <c r="K22" t="s">
         <v>70</v>
       </c>
@@ -1326,7 +1382,7 @@
         <v>10</v>
       </c>
       <c r="L24">
-        <f>(K24-I16)/($L$22*F16*0.5-E31*$M$22)</f>
+        <f>(K24-I17)/($L$22*F17*0.5-E31*$M$22)</f>
         <v>8461.3569594443834</v>
       </c>
       <c r="M24">
@@ -1343,15 +1399,15 @@
         <v>100</v>
       </c>
       <c r="L25">
-        <f t="shared" ref="L25:L28" si="6">(K25-I17)/($L$22*F17*0.5-E32*$M$22)</f>
+        <f>(K25-I19)/($L$22*F19*0.5-E33*$M$22)</f>
         <v>15046.656861969494</v>
       </c>
       <c r="M25">
-        <f t="shared" ref="M25:M28" si="7">20*L25</f>
+        <f t="shared" ref="M25:M28" si="4">20*L25</f>
         <v>300933.13723938988</v>
       </c>
       <c r="N25">
-        <f t="shared" ref="N25:N28" si="8">M25/24000</f>
+        <f t="shared" ref="N25:N28" si="5">M25/24000</f>
         <v>12.538880718307912</v>
       </c>
     </row>
@@ -1360,15 +1416,15 @@
         <v>200</v>
       </c>
       <c r="L26">
-        <f t="shared" si="6"/>
+        <f>(K26-I20)/($L$22*F20*0.5-E34*$M$22)</f>
         <v>17893.591397258639</v>
       </c>
       <c r="M26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>357871.82794517279</v>
       </c>
       <c r="N26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>14.911326164382199</v>
       </c>
     </row>
@@ -1377,15 +1433,15 @@
         <v>350</v>
       </c>
       <c r="L27">
-        <f t="shared" si="6"/>
+        <f>(K27-I21)/($L$22*F21*0.5-E35*$M$22)</f>
         <v>20580.552432645625</v>
       </c>
       <c r="M27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>411611.04865291249</v>
       </c>
       <c r="N27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>17.15046036053802</v>
       </c>
     </row>
@@ -1394,15 +1450,15 @@
         <v>500</v>
       </c>
       <c r="L28">
-        <f t="shared" si="6"/>
+        <f>(K28-I22)/($L$22*F22*0.5-E36*$M$22)</f>
         <v>22500</v>
       </c>
       <c r="M28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>450000</v>
       </c>
       <c r="N28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>18.75</v>
       </c>
     </row>
@@ -1433,7 +1489,7 @@
         <v>10</v>
       </c>
       <c r="C31">
-        <f>C32*(B31/B32)^(3/4)</f>
+        <f>C33*(B31/B33)^(3/4)</f>
         <v>0.79774438454174856</v>
       </c>
       <c r="D31">
@@ -1451,106 +1507,127 @@
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B32">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C32">
-        <f>C33*(B32/B33)^(3/4)</f>
-        <v>4.4860463436636628</v>
+        <f>C34*(B32/B34)^(3/4)</f>
+        <v>2.6674191150583848</v>
       </c>
       <c r="D32">
-        <f t="shared" ref="D32" si="9">C32/B32</f>
-        <v>4.4860463436636626E-2</v>
+        <f t="shared" ref="D32:D33" si="6">C32/B32</f>
+        <v>5.3348382301167695E-2</v>
       </c>
       <c r="E32">
         <f>C32*$K$4/$L$4/(20*60)</f>
-        <v>1.4953487812212208E-3</v>
+        <v>8.8913970501946159E-4</v>
       </c>
       <c r="F32">
         <f>B32/2/E32/(60*20)</f>
-        <v>27.864179374017578</v>
+        <v>23.430888549597874</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C33">
-        <f>$C$35*(B33/$B$35)^(3/4)</f>
-        <v>7.5446005780976142</v>
+        <f>C34*(B33/B34)^(3/4)</f>
+        <v>4.4860463436636628</v>
       </c>
       <c r="D33">
-        <f>C33/B33</f>
-        <v>3.7723002890488071E-2</v>
+        <f t="shared" si="6"/>
+        <v>4.4860463436636626E-2</v>
       </c>
       <c r="E33">
         <f>C33*$K$4/$L$4/(20*60)</f>
-        <v>2.514866859365872E-3</v>
+        <v>1.4953487812212208E-3</v>
       </c>
       <c r="F33">
         <f>B33/2/E33/(60*20)</f>
-        <v>33.136280365293764</v>
+        <v>27.864179374017578</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34">
-        <v>350</v>
+        <v>200</v>
       </c>
       <c r="C34">
-        <f>$C$35*(B34/$B$35)^(3/4)</f>
-        <v>11.479283696255481</v>
+        <f>$C$36*(B34/$B$36)^(3/4)</f>
+        <v>7.5446005780976142</v>
       </c>
       <c r="D34">
         <f>C34/B34</f>
-        <v>3.2797953417872804E-2</v>
+        <v>3.7723002890488071E-2</v>
       </c>
       <c r="E34">
         <f>C34*$K$4/$L$4/(20*60)</f>
-        <v>3.8264278987518267E-3</v>
+        <v>2.514866859365872E-3</v>
       </c>
       <c r="F34">
         <f>B34/2/E34/(60*20)</f>
-        <v>38.112134134528937</v>
+        <v>33.136280365293764</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35">
-        <v>500</v>
+        <v>350</v>
       </c>
       <c r="C35">
-        <f>B35*D35</f>
-        <v>15</v>
-      </c>
-      <c r="D35" s="2">
-        <v>0.03</v>
+        <f>$C$36*(B35/$B$36)^(3/4)</f>
+        <v>11.479283696255481</v>
+      </c>
+      <c r="D35">
+        <f>C35/B35</f>
+        <v>3.2797953417872804E-2</v>
       </c>
       <c r="E35">
         <f>C35*$K$4/$L$4/(20*60)</f>
-        <v>5.0000000000000001E-3</v>
+        <v>3.8264278987518267E-3</v>
       </c>
       <c r="F35">
         <f>B35/2/E35/(60*20)</f>
+        <v>38.112134134528937</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>500</v>
+      </c>
+      <c r="C36">
+        <f>B36*D36</f>
+        <v>15</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="E36">
+        <f>C36*$K$4/$L$4/(20*60)</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F36">
+        <f>B36/2/E36/(60*20)</f>
         <v>41.666666666666664</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
-        <v>16</v>
-      </c>
-      <c r="C37" t="s">
-        <v>17</v>
-      </c>
-      <c r="D37" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
         <v>14</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>15</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1744,4 +1821,17 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>